<commit_message>
Update Job_DS_to_Excel and Job_DS_to_sql functions
</commit_message>
<xml_diff>
--- a/Output/SQL_Docx/JOB nghiệp vụ 2.11_SQLs.xlsx
+++ b/Output/SQL_Docx/JOB nghiệp vụ 2.11_SQLs.xlsx
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Quy tắc lấy dữ liệu</t>
+          <t>2.6.2. Quy tắc lấy dữ liệu</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Bước 1 : Lấy dữ liệu kỳ đánh giá thỏa mãn điều kiện đánh giá :</t>
+          <t xml:space="preserve"> Bước 1 : Lấy dữ liệu kỳ đánh giá thỏa mãn điều kiện đánh giá :</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -556,7 +556,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>B2.1 Lấy dữ liệu kỳ trước :</t>
+          <t xml:space="preserve"> B2.1 Lấy dữ liệu kỳ trước :</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -576,7 +576,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>B2.2 Truy vấn thông tin ngày quá hạn (NO_DAY_OVERDUE	) và check vi phạm quy tắc nghị quyết</t>
+          <t xml:space="preserve"> B2.2 Truy vấn thông tin ngày quá hạn (NO_DAY_OVERDUE	) và check vi phạm quy tắc nghị quyết</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -591,7 +591,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện đánh giá</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện đánh giá</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -619,7 +619,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -645,7 +645,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -671,7 +671,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -694,7 +694,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -717,7 +717,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -740,7 +740,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -763,7 +763,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -786,7 +786,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -809,7 +809,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -832,7 +832,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -855,7 +855,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -901,7 +901,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -924,7 +924,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -947,7 +947,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -969,7 +969,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -991,7 +991,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1049,7 +1049,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1096,7 +1096,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1143,7 +1143,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1165,7 +1165,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1180,7 +1180,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1204,7 +1204,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
+          <t xml:space="preserve"> Tính doanh số giải ngân, doanh số thu gốc và lãi, doanh số phát hành LC, doanh số phát hành bảo lãnh</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1219,7 +1219,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Đánh giá tổng hợp các điều kiện trên</t>
+          <t xml:space="preserve"> Đánh giá tổng hợp các điều kiện trên</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1244,7 +1244,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Đánh giá tổng hợp các điều kiện trên</t>
+          <t xml:space="preserve"> Đánh giá tổng hợp các điều kiện trên</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1266,7 +1266,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Đánh giá tổng hợp các điều kiện trên</t>
+          <t xml:space="preserve"> Đánh giá tổng hợp các điều kiện trên</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1283,7 +1283,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1317,7 +1317,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1346,7 +1346,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1363,7 +1363,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1391,7 +1391,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1406,7 +1406,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1421,7 +1421,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1443,7 +1443,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1469,7 +1469,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Trương hợp GROUP_CONTRACT_CONDITION = PERIODIC</t>
+          <t xml:space="preserve"> Trương hợp GROUP_CONTRACT_CONDITION = PERIODIC</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1484,7 +1484,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Trường hợp GROUP_CONTRACT_CONDITION = LOAN_PRODUCT_CONDITION</t>
+          <t xml:space="preserve"> Trường hợp GROUP_CONTRACT_CONDITION = LOAN_PRODUCT_CONDITION</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1499,7 +1499,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Mô tả nghiệp vụ</t>
+          <t>3.9.3. Mô tả nghiệp vụ</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1519,7 +1519,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1543,7 +1543,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1564,7 +1564,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1579,7 +1579,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1600,7 +1600,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Sinh kỳ TSBD</t>
+          <t xml:space="preserve"> Sinh kỳ TSBD</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1615,7 +1615,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1640,7 +1640,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1661,7 +1661,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1682,7 +1682,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1701,7 +1701,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1720,7 +1720,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1742,7 +1742,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1785,7 +1785,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1832,7 +1832,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1852,7 +1852,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1880,7 +1880,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1895,7 +1895,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1927,7 +1927,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1961,7 +1961,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1976,7 +1976,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1996,7 +1996,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2017,7 +2017,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2036,7 +2036,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2063,7 +2063,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2110,7 +2110,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2144,7 +2144,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2159,7 +2159,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2174,7 +2174,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2194,7 +2194,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2213,7 +2213,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2267,7 +2267,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2292,7 +2292,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2317,7 +2317,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2337,7 +2337,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2370,7 +2370,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2390,7 +2390,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2413,7 +2413,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2428,7 +2428,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2457,7 +2457,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2477,7 +2477,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu tài sản bảo đảm</t>
+          <t xml:space="preserve"> Lấy dữ liệu tài sản bảo đảm</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2492,7 +2492,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu những hợp đồng giải ngân tương ứng</t>
+          <t xml:space="preserve"> Lấy dữ liệu những hợp đồng giải ngân tương ứng</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2513,7 +2513,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu những hợp đồng giải ngân tương ứng</t>
+          <t xml:space="preserve"> Lấy dữ liệu những hợp đồng giải ngân tương ứng</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2529,7 +2529,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu cấu hình chế tài TSBD tương ứng</t>
+          <t xml:space="preserve"> Lấy dữ liệu cấu hình chế tài TSBD tương ứng</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2550,7 +2550,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu cấu hình chế tài TSBD tương ứng</t>
+          <t xml:space="preserve"> Lấy dữ liệu cấu hình chế tài TSBD tương ứng</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2572,7 +2572,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu cấu hình chế tài TSBD tương ứng</t>
+          <t xml:space="preserve"> Lấy dữ liệu cấu hình chế tài TSBD tương ứng</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2593,7 +2593,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Tạo dữ liệu áp chế tài</t>
+          <t xml:space="preserve"> Tạo dữ liệu áp chế tài</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -2619,7 +2619,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Tạo dữ liệu áp chế tài</t>
+          <t xml:space="preserve"> Tạo dữ liệu áp chế tài</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -2645,7 +2645,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Tạo dữ liệu áp chế tài</t>
+          <t xml:space="preserve"> Tạo dữ liệu áp chế tài</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -2661,7 +2661,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Tạo dữ liệu áp chế tài</t>
+          <t xml:space="preserve"> Tạo dữ liệu áp chế tài</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -2676,7 +2676,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Tạo dữ liệu áp chế tài</t>
+          <t xml:space="preserve"> Tạo dữ liệu áp chế tài</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2706,7 +2706,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Tạo dữ liệu áp chế tài</t>
+          <t xml:space="preserve"> Tạo dữ liệu áp chế tài</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2726,7 +2726,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Tạo dữ liệu áp chế tài</t>
+          <t xml:space="preserve"> Tạo dữ liệu áp chế tài</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2741,7 +2741,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Quy tắc xử lý dữ liệu</t>
+          <t>3.16.3. Quy tắc xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2757,7 +2757,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Xử lý và cập nhật dữ liệu báo cáo KPI theo từng đơn vị</t>
+          <t xml:space="preserve"> Xử lý và cập nhật dữ liệu báo cáo KPI theo từng đơn vị</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2777,7 +2777,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Xử lý và cập nhật dữ liệu báo cáo KPI theo từng đơn vị</t>
+          <t xml:space="preserve"> Xử lý và cập nhật dữ liệu báo cáo KPI theo từng đơn vị</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Tính và lưu dữ liệu KPI với trường hợp không có dữ liệu KPI trong năm</t>
+          <t xml:space="preserve"> Tính và lưu dữ liệu KPI với trường hợp không có dữ liệu KPI trong năm</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2816,7 +2816,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Tính và lưu dữ liệu KPI với trường hợp có dữ liệu KPI trong năm</t>
+          <t xml:space="preserve"> Tính và lưu dữ liệu KPI với trường hợp có dữ liệu KPI trong năm</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2832,7 +2832,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Tính và lưu dữ liệu KPI với trường hợp có dữ liệu KPI trong năm</t>
+          <t xml:space="preserve"> Tính và lưu dữ liệu KPI với trường hợp có dữ liệu KPI trong năm</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2847,7 +2847,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Tính và lưu dữ liệu KPI với trường hợp có dữ liệu KPI trong năm</t>
+          <t xml:space="preserve"> Tính và lưu dữ liệu KPI với trường hợp có dữ liệu KPI trong năm</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2862,7 +2862,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2917,7 +2917,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2940,7 +2940,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -2955,7 +2955,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2985,7 +2985,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3002,7 +3002,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3057,7 +3057,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3112,7 +3112,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3167,7 +3167,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3222,7 +3222,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3277,7 +3277,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3330,7 +3330,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -3352,7 +3352,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -3367,7 +3367,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3397,7 +3397,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3414,7 +3414,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Lấy dữ liệu thỏa mãn điều kiện</t>
+          <t xml:space="preserve"> Lấy dữ liệu thỏa mãn điều kiện</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3429,7 +3429,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -3444,7 +3444,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3466,7 +3466,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Xử lý dữ liệu</t>
+          <t xml:space="preserve"> Xử lý dữ liệu</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">

</xml_diff>